<commit_message>
Protocol Cleanups in progress
</commit_message>
<xml_diff>
--- a/Tests/GLSeq Testing Combinations.xlsx
+++ b/Tests/GLSeq Testing Combinations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlampe\Documents\GitHub\GLSeq2\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlampe\Desktop\GLSeq2-master\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -458,11 +458,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="46188416"/>
-        <c:axId val="46189536"/>
+        <c:axId val="31603952"/>
+        <c:axId val="31605072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46188416"/>
+        <c:axId val="31603952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46189536"/>
+        <c:crossAx val="31605072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -512,7 +512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46189536"/>
+        <c:axId val="31605072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46188416"/>
+        <c:crossAx val="31603952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1667,7 +1667,7 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,7 +1850,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1859,15 +1859,15 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="12"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="12"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -1876,14 +1876,14 @@
       <c r="C18" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1893,15 +1893,15 @@
       <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="12"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="12"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -2098,8 +2098,8 @@
       <c r="C32" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="16"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
@@ -2127,8 +2127,8 @@
       <c r="D33" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="16"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -2156,8 +2156,8 @@
       <c r="D34" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="16"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>

</xml_diff>